<commit_message>
updated SIL+AUC database  data
</commit_message>
<xml_diff>
--- a/data/escapement/prelim-inseason/AUC_DataAnalysisTable_area20_2024.xlsx
+++ b/data/escapement/prelim-inseason/AUC_DataAnalysisTable_area20_2024.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\data\escapement\prelim-inseason\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\data\escapement\prelim-inseason\"/>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF436ED3-2E2D-43D8-BDAD-F640C5BF4791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AUC_DataAnalysisTable" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" r:id="rId1" name="AUC_DataAnalysisTable"/>
+    <sheet r:id="rId5" name="AUC_DataAnalysisTable1" sheetId="2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames>
+    <definedName name="AUC_DataAnalysisTable">'AUC_DataAnalysisTable1'!$A$1:$AC$36</definedName>
+  </definedNames>
+  <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
@@ -444,6 +444,10 @@
     </xf>
     <xf numFmtId="10" fontId="7" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyProtection="1" applyNumberFormat="1" xfId="0">
+      <alignment wrapText="0" vertical="center" horizontal="general"/>
+      <protection locked="1" hidden="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3092,4 +3096,2968 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Section_AreaInspected</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>SDate</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>WatershedCode</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>ShortMethod</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>ShortSpecies</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>WaterTemperature</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>Method</t>
+        </is>
+      </c>
+      <c r="I1" s="0" t="inlineStr">
+        <is>
+          <t>WaterClarity</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>Bankfull</t>
+        </is>
+      </c>
+      <c r="K1" s="0" t="inlineStr">
+        <is>
+          <t>LongSpecies</t>
+        </is>
+      </c>
+      <c r="L1" s="0" t="inlineStr">
+        <is>
+          <t>LiveAdults</t>
+        </is>
+      </c>
+      <c r="M1" s="0" t="inlineStr">
+        <is>
+          <t>DeadAdults</t>
+        </is>
+      </c>
+      <c r="N1" s="0" t="inlineStr">
+        <is>
+          <t>TotalAdults</t>
+        </is>
+      </c>
+      <c r="O1" s="0" t="inlineStr">
+        <is>
+          <t>LiveJacks</t>
+        </is>
+      </c>
+      <c r="P1" s="0" t="inlineStr">
+        <is>
+          <t>DeadJacks</t>
+        </is>
+      </c>
+      <c r="Q1" s="0" t="inlineStr">
+        <is>
+          <t>TotalJacks</t>
+        </is>
+      </c>
+      <c r="R1" s="0" t="inlineStr">
+        <is>
+          <t>PctNewFish</t>
+        </is>
+      </c>
+      <c r="S1" s="0" t="inlineStr">
+        <is>
+          <t>PctPaired</t>
+        </is>
+      </c>
+      <c r="T1" s="0" t="inlineStr">
+        <is>
+          <t>OverallReliability</t>
+        </is>
+      </c>
+      <c r="U1" s="0" t="inlineStr">
+        <is>
+          <t>EstPctSeen</t>
+        </is>
+      </c>
+      <c r="V1" s="0" t="inlineStr">
+        <is>
+          <t>FabricatedZero</t>
+        </is>
+      </c>
+      <c r="W1" s="0" t="inlineStr">
+        <is>
+          <t>ObsEfficiency</t>
+        </is>
+      </c>
+      <c r="X1" s="0" t="inlineStr">
+        <is>
+          <t>ExpLiveAdults</t>
+        </is>
+      </c>
+      <c r="Y1" s="0" t="inlineStr">
+        <is>
+          <t>ExpDeadAdults</t>
+        </is>
+      </c>
+      <c r="Z1" s="0" t="inlineStr">
+        <is>
+          <t>ExpLiveJacks</t>
+        </is>
+      </c>
+      <c r="AA1" s="0" t="inlineStr">
+        <is>
+          <t>ExpDeadJacks</t>
+        </is>
+      </c>
+      <c r="AB1" s="0" t="inlineStr">
+        <is>
+          <t>CreationDate</t>
+        </is>
+      </c>
+      <c r="AC1" s="0" t="inlineStr">
+        <is>
+          <t>SourceDB</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>GORDON RIVER</t>
+        </is>
+      </c>
+      <c r="C2" s="8">
+        <v>45568</v>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>930-054700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G2" s="0">
+        <v>99</v>
+      </c>
+      <c r="H2" s="0">
+        <v>3</v>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L2" s="0">
+        <v>40</v>
+      </c>
+      <c r="N2" s="0">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="0">
+        <v>0</v>
+      </c>
+      <c r="T2" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U2" s="0">
+        <v>1</v>
+      </c>
+      <c r="V2" s="0">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0">
+        <v>1</v>
+      </c>
+      <c r="X2" s="0">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC2" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>GORDON RIVER</t>
+        </is>
+      </c>
+      <c r="C3" s="8">
+        <v>45568</v>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>930-054700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G3" s="0">
+        <v>99</v>
+      </c>
+      <c r="H3" s="0">
+        <v>3</v>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L3" s="0">
+        <v>72</v>
+      </c>
+      <c r="N3" s="0">
+        <v>72</v>
+      </c>
+      <c r="Q3" s="0">
+        <v>0</v>
+      </c>
+      <c r="T3" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U3" s="0">
+        <v>1</v>
+      </c>
+      <c r="V3" s="0">
+        <v>0</v>
+      </c>
+      <c r="W3" s="0">
+        <v>1</v>
+      </c>
+      <c r="X3" s="0">
+        <v>72</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC3" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>GORDON RIVER</t>
+        </is>
+      </c>
+      <c r="C4" s="8">
+        <v>45568</v>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>930-054700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G4" s="0">
+        <v>99</v>
+      </c>
+      <c r="H4" s="0">
+        <v>3</v>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L4" s="0">
+        <v>547</v>
+      </c>
+      <c r="N4" s="0">
+        <v>547</v>
+      </c>
+      <c r="O4" s="0">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="0">
+        <v>45</v>
+      </c>
+      <c r="T4" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U4" s="0">
+        <v>1</v>
+      </c>
+      <c r="V4" s="0">
+        <v>0</v>
+      </c>
+      <c r="W4" s="0">
+        <v>1</v>
+      </c>
+      <c r="X4" s="0">
+        <v>547</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC4" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>GORDON RIVER</t>
+        </is>
+      </c>
+      <c r="C5" s="8">
+        <v>45568</v>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>930-054700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G5" s="0">
+        <v>99</v>
+      </c>
+      <c r="H5" s="0">
+        <v>3</v>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K5" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="L5" s="0">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0">
+        <v>0</v>
+      </c>
+      <c r="T5" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U5" s="0">
+        <v>1</v>
+      </c>
+      <c r="V5" s="0">
+        <v>0</v>
+      </c>
+      <c r="W5" s="0">
+        <v>1</v>
+      </c>
+      <c r="X5" s="0">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC5" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>GORDON RIVER</t>
+        </is>
+      </c>
+      <c r="C6" s="8">
+        <v>45568</v>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>930-054700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G6" s="0">
+        <v>99</v>
+      </c>
+      <c r="H6" s="0">
+        <v>3</v>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K6" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="L6" s="0">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0">
+        <v>0</v>
+      </c>
+      <c r="T6" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U6" s="0">
+        <v>1</v>
+      </c>
+      <c r="V6" s="0">
+        <v>0</v>
+      </c>
+      <c r="X6" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC6" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>HARRIS CREEK</t>
+        </is>
+      </c>
+      <c r="C7" s="8">
+        <v>45572</v>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-22100-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G7" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H7" s="0">
+        <v>3</v>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K7" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="N7" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>0</v>
+      </c>
+      <c r="V7" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC7" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>HARRIS CREEK</t>
+        </is>
+      </c>
+      <c r="C8" s="8">
+        <v>45572</v>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-22100-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G8" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H8" s="0">
+        <v>3</v>
+      </c>
+      <c r="I8" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J8" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K8" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L8" s="0">
+        <v>51</v>
+      </c>
+      <c r="N8" s="0">
+        <v>51</v>
+      </c>
+      <c r="O8" s="0">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>1</v>
+      </c>
+      <c r="T8" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U8" s="0">
+        <v>1</v>
+      </c>
+      <c r="V8" s="0">
+        <v>0</v>
+      </c>
+      <c r="W8" s="0">
+        <v>1</v>
+      </c>
+      <c r="X8" s="0">
+        <v>51</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC8" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>HARRIS CREEK</t>
+        </is>
+      </c>
+      <c r="C9" s="8">
+        <v>45572</v>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-22100-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G9" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H9" s="0">
+        <v>3</v>
+      </c>
+      <c r="I9" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J9" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K9" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L9" s="0">
+        <v>415</v>
+      </c>
+      <c r="N9" s="0">
+        <v>415</v>
+      </c>
+      <c r="O9" s="0">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>32</v>
+      </c>
+      <c r="T9" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U9" s="0">
+        <v>1</v>
+      </c>
+      <c r="V9" s="0">
+        <v>0</v>
+      </c>
+      <c r="W9" s="0">
+        <v>1</v>
+      </c>
+      <c r="X9" s="0">
+        <v>415</v>
+      </c>
+      <c r="AB9" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC9" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>HARRIS CREEK</t>
+        </is>
+      </c>
+      <c r="C10" s="8">
+        <v>45572</v>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-22100-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G10" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H10" s="0">
+        <v>3</v>
+      </c>
+      <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J10" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K10" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N10" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>0</v>
+      </c>
+      <c r="V10" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC10" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>HARRIS CREEK</t>
+        </is>
+      </c>
+      <c r="C11" s="8">
+        <v>45572</v>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-22100-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G11" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H11" s="0">
+        <v>3</v>
+      </c>
+      <c r="I11" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J11" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K11" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="N11" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="0">
+        <v>0</v>
+      </c>
+      <c r="V11" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC11" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>LENS CREEK</t>
+        </is>
+      </c>
+      <c r="C12" s="8">
+        <v>45574</v>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-25200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G12" s="0">
+        <v>10</v>
+      </c>
+      <c r="H12" s="0">
+        <v>3</v>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K12" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="N12" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="0">
+        <v>0</v>
+      </c>
+      <c r="T12" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="V12" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC12" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>LENS CREEK</t>
+        </is>
+      </c>
+      <c r="C13" s="8">
+        <v>45574</v>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-25200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G13" s="0">
+        <v>10</v>
+      </c>
+      <c r="H13" s="0">
+        <v>3</v>
+      </c>
+      <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J13" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K13" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L13" s="0">
+        <v>15</v>
+      </c>
+      <c r="N13" s="0">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="0">
+        <v>0</v>
+      </c>
+      <c r="T13" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U13" s="0">
+        <v>1</v>
+      </c>
+      <c r="V13" s="0">
+        <v>0</v>
+      </c>
+      <c r="W13" s="0">
+        <v>1</v>
+      </c>
+      <c r="X13" s="0">
+        <v>15</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC13" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>LENS CREEK</t>
+        </is>
+      </c>
+      <c r="C14" s="8">
+        <v>45574</v>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-25200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G14" s="0">
+        <v>10</v>
+      </c>
+      <c r="H14" s="0">
+        <v>3</v>
+      </c>
+      <c r="I14" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J14" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K14" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L14" s="0">
+        <v>10</v>
+      </c>
+      <c r="N14" s="0">
+        <v>10</v>
+      </c>
+      <c r="O14" s="0">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="0">
+        <v>1</v>
+      </c>
+      <c r="T14" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U14" s="0">
+        <v>1</v>
+      </c>
+      <c r="V14" s="0">
+        <v>0</v>
+      </c>
+      <c r="W14" s="0">
+        <v>1</v>
+      </c>
+      <c r="X14" s="0">
+        <v>10</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC14" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>LENS CREEK</t>
+        </is>
+      </c>
+      <c r="C15" s="8">
+        <v>45574</v>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-25200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G15" s="0">
+        <v>10</v>
+      </c>
+      <c r="H15" s="0">
+        <v>3</v>
+      </c>
+      <c r="I15" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J15" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K15" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N15" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="0">
+        <v>0</v>
+      </c>
+      <c r="V15" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC15" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>LENS CREEK</t>
+        </is>
+      </c>
+      <c r="C16" s="8">
+        <v>45574</v>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-25200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G16" s="0">
+        <v>10</v>
+      </c>
+      <c r="H16" s="0">
+        <v>3</v>
+      </c>
+      <c r="I16" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J16" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K16" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="N16" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="0">
+        <v>0</v>
+      </c>
+      <c r="V16" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC16" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="A17" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>RENFREW CREEK</t>
+        </is>
+      </c>
+      <c r="C17" s="8">
+        <v>45589</v>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-12100-05400-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G17" s="0">
+        <v>8</v>
+      </c>
+      <c r="H17" s="0">
+        <v>3</v>
+      </c>
+      <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J17" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K17" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L17" s="0">
+        <v>131</v>
+      </c>
+      <c r="M17" s="0">
+        <v>0</v>
+      </c>
+      <c r="N17" s="0">
+        <v>131</v>
+      </c>
+      <c r="Q17" s="0">
+        <v>0</v>
+      </c>
+      <c r="T17" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U17" s="0">
+        <v>1</v>
+      </c>
+      <c r="V17" s="0">
+        <v>0</v>
+      </c>
+      <c r="W17" s="0">
+        <v>1</v>
+      </c>
+      <c r="X17" s="0">
+        <v>131</v>
+      </c>
+      <c r="AB17" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC17" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>RENFREW CREEK</t>
+        </is>
+      </c>
+      <c r="C18" s="8">
+        <v>45589</v>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-12100-05400-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G18" s="0">
+        <v>8</v>
+      </c>
+      <c r="H18" s="0">
+        <v>3</v>
+      </c>
+      <c r="I18" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J18" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K18" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L18" s="0">
+        <v>9</v>
+      </c>
+      <c r="M18" s="0">
+        <v>1</v>
+      </c>
+      <c r="N18" s="0">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="0">
+        <v>0</v>
+      </c>
+      <c r="T18" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U18" s="0">
+        <v>0.150000005960464</v>
+      </c>
+      <c r="V18" s="0">
+        <v>0</v>
+      </c>
+      <c r="W18" s="0">
+        <v>1</v>
+      </c>
+      <c r="X18" s="0">
+        <v>60</v>
+      </c>
+      <c r="AB18" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC18" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="A19" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>RENFREW CREEK</t>
+        </is>
+      </c>
+      <c r="C19" s="8">
+        <v>45589</v>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-12100-05400-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G19" s="0">
+        <v>8</v>
+      </c>
+      <c r="H19" s="0">
+        <v>3</v>
+      </c>
+      <c r="I19" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J19" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K19" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L19" s="0">
+        <v>498</v>
+      </c>
+      <c r="M19" s="0">
+        <v>0</v>
+      </c>
+      <c r="N19" s="0">
+        <v>498</v>
+      </c>
+      <c r="O19" s="0">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="0">
+        <v>17</v>
+      </c>
+      <c r="T19" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U19" s="0">
+        <v>1</v>
+      </c>
+      <c r="V19" s="0">
+        <v>0</v>
+      </c>
+      <c r="W19" s="0">
+        <v>1</v>
+      </c>
+      <c r="X19" s="0">
+        <v>498</v>
+      </c>
+      <c r="AB19" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC19" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>RENFREW CREEK</t>
+        </is>
+      </c>
+      <c r="C20" s="8">
+        <v>45589</v>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-12100-05400-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G20" s="0">
+        <v>8</v>
+      </c>
+      <c r="H20" s="0">
+        <v>3</v>
+      </c>
+      <c r="I20" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J20" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K20" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N20" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="0">
+        <v>0</v>
+      </c>
+      <c r="V20" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC20" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="A21" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>RENFREW CREEK</t>
+        </is>
+      </c>
+      <c r="C21" s="8">
+        <v>45589</v>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-12100-05400-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G21" s="0">
+        <v>8</v>
+      </c>
+      <c r="H21" s="0">
+        <v>3</v>
+      </c>
+      <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J21" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K21" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="L21" s="0">
+        <v>8</v>
+      </c>
+      <c r="M21" s="0">
+        <v>0</v>
+      </c>
+      <c r="N21" s="0">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="0">
+        <v>0</v>
+      </c>
+      <c r="T21" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U21" s="0">
+        <v>1</v>
+      </c>
+      <c r="V21" s="0">
+        <v>0</v>
+      </c>
+      <c r="W21" s="0">
+        <v>1</v>
+      </c>
+      <c r="X21" s="0">
+        <v>8</v>
+      </c>
+      <c r="AB21" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC21" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="22">
+      <c r="A22" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C22" s="8">
+        <v>45567</v>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G22" s="0">
+        <v>6</v>
+      </c>
+      <c r="H22" s="0">
+        <v>3</v>
+      </c>
+      <c r="I22" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J22" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K22" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L22" s="0">
+        <v>11</v>
+      </c>
+      <c r="M22" s="0">
+        <v>0</v>
+      </c>
+      <c r="N22" s="0">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="0">
+        <v>0</v>
+      </c>
+      <c r="T22" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U22" s="0">
+        <v>1</v>
+      </c>
+      <c r="V22" s="0">
+        <v>0</v>
+      </c>
+      <c r="W22" s="0">
+        <v>1</v>
+      </c>
+      <c r="X22" s="0">
+        <v>11</v>
+      </c>
+      <c r="AB22" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC22" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="23">
+      <c r="A23" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C23" s="8">
+        <v>45567</v>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G23" s="0">
+        <v>6</v>
+      </c>
+      <c r="H23" s="0">
+        <v>3</v>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J23" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K23" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L23" s="0">
+        <v>1980</v>
+      </c>
+      <c r="M23" s="0">
+        <v>190</v>
+      </c>
+      <c r="N23" s="0">
+        <v>2170</v>
+      </c>
+      <c r="O23" s="0">
+        <v>44</v>
+      </c>
+      <c r="Q23" s="0">
+        <v>44</v>
+      </c>
+      <c r="T23" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U23" s="0">
+        <v>1</v>
+      </c>
+      <c r="V23" s="0">
+        <v>0</v>
+      </c>
+      <c r="W23" s="0">
+        <v>0.963503658771515</v>
+      </c>
+      <c r="X23" s="0">
+        <v>2055</v>
+      </c>
+      <c r="AB23" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC23" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="24">
+      <c r="A24" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C24" s="8">
+        <v>45567</v>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G24" s="0">
+        <v>6</v>
+      </c>
+      <c r="H24" s="0">
+        <v>3</v>
+      </c>
+      <c r="I24" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J24" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K24" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L24" s="0">
+        <v>1726</v>
+      </c>
+      <c r="M24" s="0">
+        <v>0</v>
+      </c>
+      <c r="N24" s="0">
+        <v>1726</v>
+      </c>
+      <c r="O24" s="0">
+        <v>60</v>
+      </c>
+      <c r="Q24" s="0">
+        <v>60</v>
+      </c>
+      <c r="T24" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U24" s="0">
+        <v>1</v>
+      </c>
+      <c r="V24" s="0">
+        <v>0</v>
+      </c>
+      <c r="W24" s="0">
+        <v>0.954645991325378</v>
+      </c>
+      <c r="X24" s="0">
+        <v>1808</v>
+      </c>
+      <c r="AB24" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC24" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="25">
+      <c r="A25" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C25" s="8">
+        <v>45567</v>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G25" s="0">
+        <v>6</v>
+      </c>
+      <c r="H25" s="0">
+        <v>3</v>
+      </c>
+      <c r="I25" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J25" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K25" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="L25" s="0">
+        <v>1</v>
+      </c>
+      <c r="N25" s="0">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="0">
+        <v>0</v>
+      </c>
+      <c r="T25" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U25" s="0">
+        <v>1</v>
+      </c>
+      <c r="V25" s="0">
+        <v>0</v>
+      </c>
+      <c r="W25" s="0">
+        <v>1</v>
+      </c>
+      <c r="X25" s="0">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC25" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="26">
+      <c r="A26" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C26" s="8">
+        <v>45567</v>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G26" s="0">
+        <v>6</v>
+      </c>
+      <c r="H26" s="0">
+        <v>3</v>
+      </c>
+      <c r="I26" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J26" s="0" t="inlineStr">
+        <is>
+          <t>Extremely Low</t>
+        </is>
+      </c>
+      <c r="K26" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="L26" s="0">
+        <v>6</v>
+      </c>
+      <c r="M26" s="0">
+        <v>0</v>
+      </c>
+      <c r="N26" s="0">
+        <v>6</v>
+      </c>
+      <c r="O26" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="0">
+        <v>0</v>
+      </c>
+      <c r="T26" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U26" s="0">
+        <v>0.800000011920929</v>
+      </c>
+      <c r="V26" s="0">
+        <v>0</v>
+      </c>
+      <c r="W26" s="0">
+        <v>1</v>
+      </c>
+      <c r="X26" s="0">
+        <v>8</v>
+      </c>
+      <c r="AB26" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC26" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="27">
+      <c r="A27" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C27" s="8">
+        <v>45575</v>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G27" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H27" s="0">
+        <v>3</v>
+      </c>
+      <c r="I27" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J27" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K27" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L27" s="0">
+        <v>29</v>
+      </c>
+      <c r="N27" s="0">
+        <v>29</v>
+      </c>
+      <c r="Q27" s="0">
+        <v>0</v>
+      </c>
+      <c r="T27" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U27" s="0">
+        <v>1</v>
+      </c>
+      <c r="V27" s="0">
+        <v>0</v>
+      </c>
+      <c r="W27" s="0">
+        <v>1</v>
+      </c>
+      <c r="X27" s="0">
+        <v>29</v>
+      </c>
+      <c r="AB27" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC27" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="28">
+      <c r="A28" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C28" s="8">
+        <v>45575</v>
+      </c>
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E28" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F28" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G28" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H28" s="0">
+        <v>3</v>
+      </c>
+      <c r="I28" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J28" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K28" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L28" s="0">
+        <v>287</v>
+      </c>
+      <c r="M28" s="0">
+        <v>373</v>
+      </c>
+      <c r="N28" s="0">
+        <v>660</v>
+      </c>
+      <c r="Q28" s="0">
+        <v>0</v>
+      </c>
+      <c r="T28" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U28" s="0">
+        <v>1</v>
+      </c>
+      <c r="V28" s="0">
+        <v>0</v>
+      </c>
+      <c r="W28" s="0">
+        <v>0.982876718044281</v>
+      </c>
+      <c r="X28" s="0">
+        <v>292</v>
+      </c>
+      <c r="AB28" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC28" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="29">
+      <c r="A29" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C29" s="8">
+        <v>45575</v>
+      </c>
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E29" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F29" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G29" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H29" s="0">
+        <v>3</v>
+      </c>
+      <c r="I29" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J29" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K29" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L29" s="0">
+        <v>2251</v>
+      </c>
+      <c r="N29" s="0">
+        <v>2251</v>
+      </c>
+      <c r="O29" s="0">
+        <v>209</v>
+      </c>
+      <c r="Q29" s="0">
+        <v>209</v>
+      </c>
+      <c r="T29" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U29" s="0">
+        <v>1</v>
+      </c>
+      <c r="V29" s="0">
+        <v>0</v>
+      </c>
+      <c r="W29" s="0">
+        <v>0.97319495677948</v>
+      </c>
+      <c r="X29" s="0">
+        <v>2313</v>
+      </c>
+      <c r="AB29" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC29" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="30">
+      <c r="A30" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C30" s="8">
+        <v>45575</v>
+      </c>
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E30" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F30" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G30" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H30" s="0">
+        <v>3</v>
+      </c>
+      <c r="I30" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J30" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K30" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N30" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="0">
+        <v>0</v>
+      </c>
+      <c r="V30" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC30" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="31">
+      <c r="A31" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C31" s="8">
+        <v>45575</v>
+      </c>
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E31" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F31" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G31" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="H31" s="0">
+        <v>3</v>
+      </c>
+      <c r="I31" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J31" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K31" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="L31" s="0">
+        <v>16</v>
+      </c>
+      <c r="N31" s="0">
+        <v>16</v>
+      </c>
+      <c r="Q31" s="0">
+        <v>0</v>
+      </c>
+      <c r="T31" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U31" s="0">
+        <v>0.899999976158142</v>
+      </c>
+      <c r="V31" s="0">
+        <v>0</v>
+      </c>
+      <c r="W31" s="0">
+        <v>1</v>
+      </c>
+      <c r="X31" s="0">
+        <v>18</v>
+      </c>
+      <c r="AB31" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC31" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="32">
+      <c r="A32" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C32" s="8">
+        <v>45590</v>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E32" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F32" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G32" s="0">
+        <v>8</v>
+      </c>
+      <c r="H32" s="0">
+        <v>3</v>
+      </c>
+      <c r="I32" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J32" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K32" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L32" s="0">
+        <v>370</v>
+      </c>
+      <c r="N32" s="0">
+        <v>370</v>
+      </c>
+      <c r="Q32" s="0">
+        <v>0</v>
+      </c>
+      <c r="T32" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U32" s="0">
+        <v>0.600000023841858</v>
+      </c>
+      <c r="V32" s="0">
+        <v>0</v>
+      </c>
+      <c r="W32" s="0">
+        <v>1</v>
+      </c>
+      <c r="X32" s="0">
+        <v>617</v>
+      </c>
+      <c r="AB32" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC32" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="33">
+      <c r="A33" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C33" s="8">
+        <v>45590</v>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E33" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F33" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G33" s="0">
+        <v>8</v>
+      </c>
+      <c r="H33" s="0">
+        <v>3</v>
+      </c>
+      <c r="I33" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J33" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K33" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L33" s="0">
+        <v>2</v>
+      </c>
+      <c r="M33" s="0">
+        <v>2</v>
+      </c>
+      <c r="N33" s="0">
+        <v>4</v>
+      </c>
+      <c r="Q33" s="0">
+        <v>0</v>
+      </c>
+      <c r="T33" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U33" s="0">
+        <v>0.300000011920929</v>
+      </c>
+      <c r="V33" s="0">
+        <v>0</v>
+      </c>
+      <c r="W33" s="0">
+        <v>1</v>
+      </c>
+      <c r="X33" s="0">
+        <v>7</v>
+      </c>
+      <c r="AB33" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC33" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="34">
+      <c r="A34" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C34" s="8">
+        <v>45590</v>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E34" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F34" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G34" s="0">
+        <v>8</v>
+      </c>
+      <c r="H34" s="0">
+        <v>3</v>
+      </c>
+      <c r="I34" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J34" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K34" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L34" s="0">
+        <v>108</v>
+      </c>
+      <c r="N34" s="0">
+        <v>108</v>
+      </c>
+      <c r="Q34" s="0">
+        <v>0</v>
+      </c>
+      <c r="T34" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U34" s="0">
+        <v>1</v>
+      </c>
+      <c r="V34" s="0">
+        <v>0</v>
+      </c>
+      <c r="W34" s="0">
+        <v>1</v>
+      </c>
+      <c r="X34" s="0">
+        <v>108</v>
+      </c>
+      <c r="AB34" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC34" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="35">
+      <c r="A35" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C35" s="8">
+        <v>45590</v>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E35" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F35" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G35" s="0">
+        <v>8</v>
+      </c>
+      <c r="H35" s="0">
+        <v>3</v>
+      </c>
+      <c r="I35" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J35" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K35" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N35" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="0">
+        <v>0</v>
+      </c>
+      <c r="V35" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC35" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="36">
+      <c r="A36" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>SAN JUAN RIVER</t>
+        </is>
+      </c>
+      <c r="C36" s="8">
+        <v>45590</v>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>930-053800-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E36" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F36" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G36" s="0">
+        <v>8</v>
+      </c>
+      <c r="H36" s="0">
+        <v>3</v>
+      </c>
+      <c r="I36" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J36" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K36" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="N36" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="0">
+        <v>0</v>
+      </c>
+      <c r="T36" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U36" s="0">
+        <v>1</v>
+      </c>
+      <c r="V36" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="8">
+        <v>45622.4991203704</v>
+      </c>
+      <c r="AC36" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>